<commit_message>
Integracion todo el proyecto
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8469C4A-224C-4796-AAD2-67D60C61070E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF684285-3893-46C5-B275-5DF72295E006}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="11205" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4695" yWindow="2340" windowWidth="21600" windowHeight="11205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
   <si>
     <t>Key</t>
   </si>
@@ -205,6 +205,12 @@
   </si>
   <si>
     <t>Cola</t>
+  </si>
+  <si>
+    <t>URLEndpoint</t>
+  </si>
+  <si>
+    <t>Url del endpoint</t>
   </si>
 </sst>
 </file>
@@ -545,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -767,11 +773,23 @@
         <v>59</v>
       </c>
     </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
     <hyperlink ref="B14" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B20" r:id="rId4" xr:uid="{5B045024-C257-42E3-B4EA-166A89B1334E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -781,7 +799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C65160-A8E0-446E-AF4F-971CC91598A3}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>

</xml_diff>